<commit_message>
minor update on which columns to show in table 1 and supptable1
</commit_message>
<xml_diff>
--- a/assets/table1_metadata.xlsx
+++ b/assets/table1_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siyuan/Dropbox (Harvard University)/ibd_paper/tables/table1/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siyuan/Dropbox (Harvard University)/ibd_paper/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E97B2099-F8C4-0E4E-BAEC-2142BEBCB077}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF230C0-B7DD-9E44-B058-26AE14D130C8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" activeTab="1"/>
+    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table1_metadata" sheetId="1" r:id="rId1"/>
@@ -392,7 +392,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1246,11 +1246,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1355,6 +1355,9 @@
       <c r="A4" t="s">
         <v>24</v>
       </c>
+      <c r="B4">
+        <v>31142855</v>
+      </c>
       <c r="C4" t="s">
         <v>25</v>
       </c>
@@ -1602,11 +1605,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1642,6 +1645,9 @@
       <c r="A4" t="s">
         <v>24</v>
       </c>
+      <c r="B4">
+        <v>31142855</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1708,8 +1714,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" r:id="rId1" location="R28" display="https://www-ncbi-nlm-nih-gov.ezp-prod1.hul.harvard.edu/pmc/articles/PMC5319707/ - R28"/>
-    <hyperlink ref="D9" r:id="rId2" location="R29" display="https://www-ncbi-nlm-nih-gov.ezp-prod1.hul.harvard.edu/pmc/articles/PMC5319707/ - R29"/>
+    <hyperlink ref="C9" r:id="rId1" location="R28" display="https://www-ncbi-nlm-nih-gov.ezp-prod1.hul.harvard.edu/pmc/articles/PMC5319707/ - R28" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D9" r:id="rId2" location="R29" display="https://www-ncbi-nlm-nih-gov.ezp-prod1.hul.harvard.edu/pmc/articles/PMC5319707/ - R29" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>